<commit_message>
fixed for current strategy
</commit_message>
<xml_diff>
--- a/prerequisite.xlsx
+++ b/prerequisite.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak M\Downloads\Zerodha Trading\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerodha\Zerodha-Trading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7617D41-143F-4179-8BFA-45942D4C6FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1D9154-6FD8-4C40-9485-9290F67F33B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3408" windowWidth="17280" windowHeight="8832" xr2:uid="{C7E1F6E9-B546-4A97-954C-C86DE5D28C97}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C7E1F6E9-B546-4A97-954C-C86DE5D28C97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Lotsize</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Minutes</t>
   </si>
@@ -54,6 +51,15 @@
   </si>
   <si>
     <t>NIFTY 50</t>
+  </si>
+  <si>
+    <t>24JUL2024</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>LotSize</t>
   </si>
 </sst>
 </file>
@@ -97,9 +103,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,46 +448,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2AD667-81BC-4A6D-A63F-CCFC531DBB56}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3000</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>